<commit_message>
Création publication-request et correction index.html 4d38b01f68c1d20ab9a1a6af24b69df09cc87189
</commit_message>
<xml_diff>
--- a/concertation/ig/StructureDefinition-TDEBundleResultatReponseRechercheTraces.xlsx
+++ b/concertation/ig/StructureDefinition-TDEBundleResultatReponseRechercheTraces.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>2.0.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-02-06T14:02:29+00:00</t>
+    <t>2026-02-06T14:23:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>